<commit_message>
mobile responsive feature added
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ozodorifjonov/Desktop/projects/FREELANCING/tangem-test-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42914FC0-76D1-F843-AB68-1F4F2582AF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62464E04-CCC3-7E43-8A8C-DF6203D65E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Key</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>ALERT.SHOP_NOW</t>
+  </si>
+  <si>
+    <t>Shop now through Monday</t>
+  </si>
+  <si>
+    <t>Делайте покупки до понедельника</t>
+  </si>
+  <si>
+    <t>CARD.SHOP_NOW_THROUGH_MONDAY</t>
   </si>
 </sst>
 </file>
@@ -476,7 +485,7 @@
   <dimension ref="A1:C162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,6 +570,17 @@
       </c>
       <c r="C7" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>